<commit_message>
Updated Code for Invoice (PO And NON-PO) and Adding Validations
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADAD09A-967D-4164-B6FD-5A1BE3FC2C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9DB5F-336F-4335-AD7B-541A5B66CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Environment</t>
   </si>
@@ -99,9 +99,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>EMEAAD\spineau</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>010</t>
   </si>
   <si>
-    <t>Test Automation India Anmol</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>PO2201000659</t>
-  </si>
-  <si>
     <t>600</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>Test Automation Non-Po India Anmol</t>
   </si>
   <si>
-    <t>EMEAAD\abouhadjer</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -166,6 +154,9 @@
   </si>
   <si>
     <t>MAINT FIXED COST</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
@@ -552,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +568,7 @@
     <col min="15" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.85546875" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
@@ -604,7 +595,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -637,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>12</v>
@@ -646,7 +637,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>15</v>
@@ -669,148 +660,75 @@
         <v>21</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="Q2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="T2" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{9C623086-8A56-4E48-956D-83C73EB2A0B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
testing for SSP Non-PO Invoice
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9DB5F-336F-4335-AD7B-541A5B66CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C3259A-5DC3-4978-B925-F06F02F2626A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>Test Automation Non-Po India Anmol</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>EMEAAD\alepicard</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>99</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,28 +693,28 @@
         <v>34</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="Q2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="V2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W2" s="13" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Change of Approver Header to Requester
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FAC38F-023D-4C60-9452-D50E7302EC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9D7074-4C78-48EF-824B-B7227A58B364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Coding</t>
   </si>
   <si>
-    <t>Approver</t>
-  </si>
-  <si>
     <t>MAINT FIXED COST</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>EMEAAD\coanea</t>
+  </si>
+  <si>
+    <t>Requester</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>15</v>
@@ -654,56 +654,56 @@
         <v>20</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="M2" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="R2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S2" s="15"/>
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
       <c r="V2" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W2" s="13" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Updating project for Invoice flow , Updated 4 Flow as adding Manual functionality for matching
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9D7074-4C78-48EF-824B-B7227A58B364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021C9867-667D-42FB-A679-682E346974F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Environment</t>
   </si>
@@ -114,46 +125,85 @@
     <t>Coding</t>
   </si>
   <si>
-    <t>MAINT FIXED COST</t>
-  </si>
-  <si>
-    <t>PO CT 5 : Hardware 362</t>
-  </si>
-  <si>
-    <t>S00001610001</t>
-  </si>
-  <si>
     <t>EMEAAD\oarsim</t>
   </si>
   <si>
-    <t>362</t>
-  </si>
-  <si>
     <t>08/06/2022</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>BED200FR</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Requester</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Manual matching</t>
+  </si>
+  <si>
+    <t>D200E</t>
+  </si>
+  <si>
+    <t>S00006662001</t>
   </si>
   <si>
     <t>1000</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>PO2236200261</t>
-  </si>
-  <si>
-    <t>EMEAAD\coanea</t>
-  </si>
-  <si>
-    <t>Requester</t>
+    <t>200</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-004</t>
+  </si>
+  <si>
+    <t>HR services - Car fleet</t>
+  </si>
+  <si>
+    <t>VEHI / MAINT / FIXED COST</t>
+  </si>
+  <si>
+    <t>EMEAAD\ehumbert</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>PO2213600592</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-001</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PO2213600593</t>
+  </si>
+  <si>
+    <t>S00000244002</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-002</t>
+  </si>
+  <si>
+    <t>PO2213600594</t>
+  </si>
+  <si>
+    <t>TESTCASE-AUTO0911-003</t>
   </si>
 </sst>
 </file>
@@ -163,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +225,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -216,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,6 +295,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -540,184 +597,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="6"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="6"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="16"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="X2" s="14" t="s">
+      <c r="W5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1EFBD0EA-5C5D-4D15-9193-570DDAA1D644}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{ACA9E775-FF4B-4CE5-B588-9AD7FD79CBB4}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{416163C3-617C-497E-AA3D-6E768404A1B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updating staleElement Exception handling for Tax Coding
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021C9867-667D-42FB-A679-682E346974F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23E0D77-2317-451C-BADE-574993BBB966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Environment</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>TESTCASE-AUTO0911-003</t>
+  </si>
+  <si>
+    <t>ehumbert</t>
   </si>
 </sst>
 </file>
@@ -599,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +968,7 @@
       </c>
       <c r="U5" s="15"/>
       <c r="V5" s="15" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="W5" s="15" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
test non po invoice
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23E0D77-2317-451C-BADE-574993BBB966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4B8541-FFE5-4A4B-B7C1-4C2439D3D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Environment</t>
   </si>
@@ -168,42 +168,6 @@
   </si>
   <si>
     <t>99</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>PO2213600592</t>
-  </si>
-  <si>
-    <t>TESTCASE-AUTO0911-001</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>PO2213600593</t>
-  </si>
-  <si>
-    <t>S00000244002</t>
-  </si>
-  <si>
-    <t>TESTCASE-AUTO0911-002</t>
-  </si>
-  <si>
-    <t>PO2213600594</t>
-  </si>
-  <si>
-    <t>TESTCASE-AUTO0911-003</t>
   </si>
   <si>
     <t>ehumbert</t>
@@ -600,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="J4" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,9 +678,7 @@
       <c r="A2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
         <v>20</v>
       </c>
@@ -729,9 +691,7 @@
       <c r="F2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="G2" s="14"/>
       <c r="H2" s="14" t="s">
         <v>25</v>
       </c>
@@ -739,257 +699,57 @@
         <v>36</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>35</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15" t="s">
-        <v>49</v>
-      </c>
+      <c r="P2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="15"/>
       <c r="R2" s="15" t="s">
         <v>31</v>
       </c>
       <c r="S2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="14" t="s">
-        <v>29</v>
+      <c r="V2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="X2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="Y2" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="X5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{1EFBD0EA-5C5D-4D15-9193-570DDAA1D644}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{ACA9E775-FF4B-4CE5-B588-9AD7FD79CBB4}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{416163C3-617C-497E-AA3D-6E768404A1B6}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{416163C3-617C-497E-AA3D-6E768404A1B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updating Output File NAme
</commit_message>
<xml_diff>
--- a/provide/test/Invoice.xlsx
+++ b/provide/test/Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anchaudhary\eclipse-workspace\Projects\Provide_Automation_Project\provide\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26CD110-EB6F-4F0C-80CE-D1A497E696AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27619047-B031-4D4A-A94D-FF90628724A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>